<commit_message>
Update Testcases Register Negative Skenario
</commit_message>
<xml_diff>
--- a/src/main/java/data/data_test.xlsx
+++ b/src/main/java/data/data_test.xlsx
@@ -2,22 +2,26 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+  <workbookPr codeName="ThisWorkbook" defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\test-web\pwa\pwa\src\main\java\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\test-web\pwa\pwa_ui_test\src\main\java\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7450" firstSheet="2" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7450" firstSheet="6" activeTab="9"/>
   </bookViews>
   <sheets>
-    <sheet name="Login_Success" sheetId="1" r:id="rId1"/>
-    <sheet name="Login_Alert_Username" sheetId="2" r:id="rId2"/>
-    <sheet name="Login_Alert_Password" sheetId="3" r:id="rId3"/>
-    <sheet name="Login_Alert_Popup" sheetId="4" r:id="rId4"/>
+    <sheet name="Login_Success" sheetId="15" r:id="rId1"/>
+    <sheet name="Login_Alert_Username" sheetId="20" r:id="rId2"/>
+    <sheet name="Login_Alert_Password" sheetId="21" r:id="rId3"/>
+    <sheet name="Login_Alert_Popup" sheetId="16" r:id="rId4"/>
     <sheet name="List_Menu_Account_Popup_Login" sheetId="12" r:id="rId5"/>
     <sheet name="List_Menu_Account_Direct" sheetId="11" r:id="rId6"/>
+    <sheet name="Register_Alert" sheetId="13" r:id="rId7"/>
+    <sheet name="Register_Email_Alert" sheetId="22" r:id="rId8"/>
+    <sheet name="Register_Password1_Alert" sheetId="23" r:id="rId9"/>
+    <sheet name="Register_Password2_Alert" sheetId="24" r:id="rId10"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -29,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="43">
   <si>
     <t>Username</t>
   </si>
@@ -82,12 +86,6 @@
     <t>628229098776544</t>
   </si>
   <si>
-    <t>Url</t>
-  </si>
-  <si>
-    <t>/login</t>
-  </si>
-  <si>
     <t>Element</t>
   </si>
   <si>
@@ -134,6 +132,36 @@
   </si>
   <si>
     <t>Faq</t>
+  </si>
+  <si>
+    <t>Email</t>
+  </si>
+  <si>
+    <t>please try again, email has been taken</t>
+  </si>
+  <si>
+    <t>rtgsfad.com</t>
+  </si>
+  <si>
+    <t>password</t>
+  </si>
+  <si>
+    <t>nteamqcdfard@gmail.com</t>
+  </si>
+  <si>
+    <t>Re Password</t>
+  </si>
+  <si>
+    <t>kurang</t>
+  </si>
+  <si>
+    <t>Password must at least 8 characters</t>
+  </si>
+  <si>
+    <t>passwordBeda</t>
+  </si>
+  <si>
+    <t>Password must match</t>
   </si>
 </sst>
 </file>
@@ -192,7 +220,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
@@ -200,7 +228,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -485,318 +512,331 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D3"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <cols>
-    <col min="1" max="1" width="5.6328125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="20.81640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.90625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.1796875" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A1" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="B1" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
-        <v>18</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
-        <v>18</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C3" t="s">
-        <v>3</v>
-      </c>
-      <c r="D3" t="s">
-        <v>6</v>
-      </c>
-    </row>
-  </sheetData>
-  <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1"/>
-  </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D3"/>
+  <sheetPr codeName="Sheet1"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="20.81640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.90625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.26953125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="37.6328125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.90625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.1796875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A3" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:D2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="23.26953125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.90625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.1796875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.26953125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="B1" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="B1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="C1" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="D1" s="4" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
-        <v>18</v>
+      <c r="A2" s="1" t="s">
+        <v>37</v>
       </c>
       <c r="B2" t="s">
-        <v>8</v>
+        <v>36</v>
       </c>
       <c r="C2" t="s">
-        <v>10</v>
+        <v>41</v>
       </c>
       <c r="D2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
-        <v>18</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C3" t="s">
-        <v>10</v>
-      </c>
-      <c r="D3" t="s">
-        <v>14</v>
+        <v>42</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection sqref="A1:C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="5.6328125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="20.81640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.26953125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="32.90625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="37.6328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A1" s="4" t="s">
-        <v>17</v>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A1" s="3" t="s">
+        <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="3" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>18</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>2</v>
+        <v>8</v>
+      </c>
+      <c r="B2" t="s">
+        <v>10</v>
       </c>
       <c r="C2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A3" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B3" t="s">
         <v>10</v>
       </c>
-      <c r="D2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
-        <v>18</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>4</v>
-      </c>
       <c r="C3" t="s">
-        <v>10</v>
-      </c>
-      <c r="D3" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="5.6328125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="22.54296875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.26953125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="25" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="32.90625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A1" s="4" t="s">
-        <v>17</v>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A1" s="3" t="s">
+        <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="3" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
-        <v>18</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>15</v>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" t="s">
+        <v>10</v>
       </c>
       <c r="C2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A3" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" t="s">
         <v>10</v>
       </c>
-      <c r="D2" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
-        <v>18</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>16</v>
-      </c>
       <c r="C3" t="s">
-        <v>10</v>
-      </c>
-      <c r="D3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1"/>
+    <hyperlink ref="A2" r:id="rId1"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C4"/>
+  <sheetPr codeName="Sheet3"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="22.54296875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.26953125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="25" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A2" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A3" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr codeName="Sheet4"/>
+  <dimension ref="A1:C4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:C1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="2" max="3" width="11.81640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A1" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="C1" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="B1" s="5" t="s">
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A2" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="B2" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="C2" s="5" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A2" s="6" t="s">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A3" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="29" x14ac:dyDescent="0.35">
+      <c r="A4" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="B2" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="C2" s="6" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A3" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="B3" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="C3" s="6" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" ht="29" x14ac:dyDescent="0.35">
-      <c r="A4" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="B4" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="C4" s="6" t="s">
-        <v>23</v>
+      <c r="B4" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>21</v>
       </c>
     </row>
   </sheetData>
@@ -806,10 +846,11 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr codeName="Sheet5"/>
   <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection sqref="A1:B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -819,46 +860,262 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A1" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="B1" s="5" t="s">
+      <c r="A1" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="B1" s="4" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B2" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B3" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B4" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B5" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr codeName="Sheet6"/>
+  <dimension ref="A1:D5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D5" sqref="A5:D5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="23.26953125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.90625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.1796875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="32.81640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A1" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" t="s">
+        <v>36</v>
+      </c>
+      <c r="C2" t="s">
+        <v>36</v>
+      </c>
+      <c r="D2" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>35</v>
+      </c>
+      <c r="B3" t="s">
+        <v>36</v>
+      </c>
+      <c r="C3" t="s">
+        <v>36</v>
+      </c>
+      <c r="D3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A4" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B4" t="s">
+        <v>39</v>
+      </c>
+      <c r="C4" t="s">
+        <v>39</v>
+      </c>
+      <c r="D4" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A5" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B5" t="s">
+        <v>36</v>
+      </c>
+      <c r="C5" t="s">
+        <v>41</v>
+      </c>
+      <c r="D5" t="s">
+        <v>42</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1"/>
+    <hyperlink ref="A4" r:id="rId2"/>
+    <hyperlink ref="A5" r:id="rId3"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId4"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G2" sqref="G2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="20.81640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.90625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.453125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="32.81640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A1" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" t="s">
+        <v>36</v>
+      </c>
+      <c r="C2" t="s">
+        <v>36</v>
+      </c>
+      <c r="D2" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>35</v>
+      </c>
+      <c r="B3" t="s">
+        <v>36</v>
+      </c>
+      <c r="C3" t="s">
+        <v>36</v>
+      </c>
+      <c r="D3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:D1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="23.26953125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.90625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.453125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="30.90625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A1" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A2" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B2" t="s">
+        <v>39</v>
+      </c>
+      <c r="C2" t="s">
+        <v>39</v>
+      </c>
+      <c r="D2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Update Textcases Register Negative Skenario
</commit_message>
<xml_diff>
--- a/src/main/java/data/data_test.xlsx
+++ b/src/main/java/data/data_test.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7450" firstSheet="6" activeTab="9"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7450" firstSheet="6" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="Login_Success" sheetId="15" r:id="rId1"/>
@@ -18,10 +18,9 @@
     <sheet name="Login_Alert_Popup" sheetId="16" r:id="rId4"/>
     <sheet name="List_Menu_Account_Popup_Login" sheetId="12" r:id="rId5"/>
     <sheet name="List_Menu_Account_Direct" sheetId="11" r:id="rId6"/>
-    <sheet name="Register_Alert" sheetId="13" r:id="rId7"/>
-    <sheet name="Register_Email_Alert" sheetId="22" r:id="rId8"/>
-    <sheet name="Register_Password1_Alert" sheetId="23" r:id="rId9"/>
-    <sheet name="Register_Password2_Alert" sheetId="24" r:id="rId10"/>
+    <sheet name="Register_Email_Alert" sheetId="22" r:id="rId7"/>
+    <sheet name="Register_Password1_Alert" sheetId="23" r:id="rId8"/>
+    <sheet name="Register_Password2_Alert" sheetId="24" r:id="rId9"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -33,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="43">
   <si>
     <t>Username</t>
   </si>
@@ -567,58 +566,6 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D2"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:D2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <cols>
-    <col min="1" max="1" width="23.26953125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.90625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.1796875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="19.26953125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A1" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="B1" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="D1" s="4" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A2" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="B2" t="s">
-        <v>36</v>
-      </c>
-      <c r="C2" t="s">
-        <v>41</v>
-      </c>
-      <c r="D2" t="s">
-        <v>42</v>
-      </c>
-    </row>
-  </sheetData>
-  <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1"/>
-  </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C3"/>
@@ -906,107 +853,9 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr codeName="Sheet6"/>
-  <dimension ref="A1:D5"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D5" sqref="A5:D5"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <cols>
-    <col min="1" max="1" width="23.26953125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.90625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.1796875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="32.81640625" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A1" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="B1" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="D1" s="4" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A2" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2" t="s">
-        <v>36</v>
-      </c>
-      <c r="C2" t="s">
-        <v>36</v>
-      </c>
-      <c r="D2" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
-        <v>35</v>
-      </c>
-      <c r="B3" t="s">
-        <v>36</v>
-      </c>
-      <c r="C3" t="s">
-        <v>36</v>
-      </c>
-      <c r="D3" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A4" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="B4" t="s">
-        <v>39</v>
-      </c>
-      <c r="C4" t="s">
-        <v>39</v>
-      </c>
-      <c r="D4" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A5" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="B5" t="s">
-        <v>36</v>
-      </c>
-      <c r="C5" t="s">
-        <v>41</v>
-      </c>
-      <c r="D5" t="s">
-        <v>42</v>
-      </c>
-    </row>
-  </sheetData>
-  <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1"/>
-    <hyperlink ref="A4" r:id="rId2"/>
-    <hyperlink ref="A5" r:id="rId3"/>
-  </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId4"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
@@ -1068,7 +917,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D2"/>
   <sheetViews>
@@ -1118,4 +967,56 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:D2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="23.26953125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.90625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.1796875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.26953125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A1" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A2" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B2" t="s">
+        <v>36</v>
+      </c>
+      <c r="C2" t="s">
+        <v>41</v>
+      </c>
+      <c r="D2" t="s">
+        <v>42</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Update TestCase Register By Phone & email Negative Skenario
</commit_message>
<xml_diff>
--- a/src/main/java/data/data_test.xlsx
+++ b/src/main/java/data/data_test.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7450" firstSheet="6" activeTab="6"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7450" firstSheet="9" activeTab="10"/>
   </bookViews>
   <sheets>
     <sheet name="Login_Success" sheetId="15" r:id="rId1"/>
@@ -19,8 +19,11 @@
     <sheet name="List_Menu_Account_Popup_Login" sheetId="12" r:id="rId5"/>
     <sheet name="List_Menu_Account_Direct" sheetId="11" r:id="rId6"/>
     <sheet name="Register_Email_Alert" sheetId="22" r:id="rId7"/>
-    <sheet name="Register_Password1_Alert" sheetId="23" r:id="rId8"/>
-    <sheet name="Register_Password2_Alert" sheetId="24" r:id="rId9"/>
+    <sheet name="Register_Password1_Alert_Email" sheetId="23" r:id="rId8"/>
+    <sheet name="Register_Password2_Alert_Email" sheetId="24" r:id="rId9"/>
+    <sheet name="Register_Password2_Alert_Phone" sheetId="26" r:id="rId10"/>
+    <sheet name="Register_Password1_Alert_Phone" sheetId="27" r:id="rId11"/>
+    <sheet name="Register_Phone_Alert" sheetId="25" r:id="rId12"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -32,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="49">
   <si>
     <t>Username</t>
   </si>
@@ -161,6 +164,24 @@
   </si>
   <si>
     <t>Password must match</t>
+  </si>
+  <si>
+    <t>Phone</t>
+  </si>
+  <si>
+    <t>00909089897897</t>
+  </si>
+  <si>
+    <t>please try again, phone has been taken</t>
+  </si>
+  <si>
+    <t>82278843303</t>
+  </si>
+  <si>
+    <t>84534343436</t>
+  </si>
+  <si>
+    <t>863436763543</t>
   </si>
 </sst>
 </file>
@@ -219,7 +240,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
@@ -230,6 +251,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -566,6 +588,173 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="11.81640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.90625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.1796875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.26953125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A1" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A2" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="B2" t="s">
+        <v>36</v>
+      </c>
+      <c r="C2" t="s">
+        <v>41</v>
+      </c>
+      <c r="D2" t="s">
+        <v>42</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1" display="nteamqcdfard@gmail.com"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="23.26953125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.90625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.453125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="30.90625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A1" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A2" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="B2" t="s">
+        <v>39</v>
+      </c>
+      <c r="C2" t="s">
+        <v>39</v>
+      </c>
+      <c r="D2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1" display="nteamqcdfard@gmail.com"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="14.90625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.90625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.453125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="37.6328125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A1" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A2" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="B2" t="s">
+        <v>36</v>
+      </c>
+      <c r="C2" t="s">
+        <v>36</v>
+      </c>
+      <c r="D2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A3" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="B3" t="s">
+        <v>36</v>
+      </c>
+      <c r="C3" t="s">
+        <v>36</v>
+      </c>
+      <c r="D3" t="s">
+        <v>45</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C3"/>
@@ -855,7 +1044,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
@@ -922,7 +1111,7 @@
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:D1"/>
+      <selection sqref="A1:D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -974,7 +1163,7 @@
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:D2"/>
+      <selection sqref="A1:D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>

<commit_message>
up new test cases exlusive, chat , mylist dll lupa
</commit_message>
<xml_diff>
--- a/src/main/java/data/data_test.xlsx
+++ b/src/main/java/data/data_test.xlsx
@@ -9,21 +9,27 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7450" firstSheet="9" activeTab="10"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7450" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Login_Success" sheetId="15" r:id="rId1"/>
-    <sheet name="Login_Alert_Username" sheetId="20" r:id="rId2"/>
-    <sheet name="Login_Alert_Password" sheetId="21" r:id="rId3"/>
-    <sheet name="Login_Alert_Popup" sheetId="16" r:id="rId4"/>
-    <sheet name="List_Menu_Account_Popup_Login" sheetId="12" r:id="rId5"/>
-    <sheet name="List_Menu_Account_Direct" sheetId="11" r:id="rId6"/>
-    <sheet name="Register_Email_Alert" sheetId="22" r:id="rId7"/>
-    <sheet name="Register_Password1_Alert_Email" sheetId="23" r:id="rId8"/>
-    <sheet name="Register_Password2_Alert_Email" sheetId="24" r:id="rId9"/>
-    <sheet name="Register_Password2_Alert_Phone" sheetId="26" r:id="rId10"/>
-    <sheet name="Register_Password1_Alert_Phone" sheetId="27" r:id="rId11"/>
-    <sheet name="Register_Phone_Alert" sheetId="25" r:id="rId12"/>
+    <sheet name="List_Share" sheetId="35" r:id="rId2"/>
+    <sheet name="Login_Alert_Username" sheetId="20" r:id="rId3"/>
+    <sheet name="Login_Alert_Password" sheetId="21" r:id="rId4"/>
+    <sheet name="Login_Alert_Popup" sheetId="16" r:id="rId5"/>
+    <sheet name="List_Menu_Account_Popup_Login" sheetId="12" r:id="rId6"/>
+    <sheet name="List_Menu_Account_Direct" sheetId="11" r:id="rId7"/>
+    <sheet name="Register_Email_Alert" sheetId="22" r:id="rId8"/>
+    <sheet name="Register_Password1_Alert_Email" sheetId="23" r:id="rId9"/>
+    <sheet name="Register_Password2_Alert_Email" sheetId="24" r:id="rId10"/>
+    <sheet name="Register_Password2_Alert_Phone" sheetId="26" r:id="rId11"/>
+    <sheet name="Register_Password1_Alert_Phone" sheetId="27" r:id="rId12"/>
+    <sheet name="Register_Phone_Alert" sheetId="25" r:id="rId13"/>
+    <sheet name="Register_List_Gender" sheetId="28" r:id="rId14"/>
+    <sheet name="Chat" sheetId="29" r:id="rId15"/>
+    <sheet name="Mylist" sheetId="30" r:id="rId16"/>
+    <sheet name="Forget_Password_Alert" sheetId="31" r:id="rId17"/>
+    <sheet name="List_Tab_Menu_Exclusive" sheetId="34" r:id="rId18"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -35,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="87">
   <si>
     <t>Username</t>
   </si>
@@ -182,12 +188,129 @@
   </si>
   <si>
     <t>863436763543</t>
+  </si>
+  <si>
+    <t>Gender</t>
+  </si>
+  <si>
+    <t>Male</t>
+  </si>
+  <si>
+    <t>Female</t>
+  </si>
+  <si>
+    <t>Live Tv</t>
+  </si>
+  <si>
+    <t>Chat Text</t>
+  </si>
+  <si>
+    <t>Selamat menonton semua!</t>
+  </si>
+  <si>
+    <t>Nickname</t>
+  </si>
+  <si>
+    <t>dikakokodikakoko</t>
+  </si>
+  <si>
+    <t>rcti</t>
+  </si>
+  <si>
+    <t>mnctv</t>
+  </si>
+  <si>
+    <t>gtv</t>
+  </si>
+  <si>
+    <t>inews</t>
+  </si>
+  <si>
+    <t>email.com</t>
+  </si>
+  <si>
+    <t>454546546565646</t>
+  </si>
+  <si>
+    <t>082222992299</t>
+  </si>
+  <si>
+    <t>iustrtqc@gmail.com</t>
+  </si>
+  <si>
+    <t>Share By</t>
+  </si>
+  <si>
+    <t>facebook</t>
+  </si>
+  <si>
+    <t>twitter</t>
+  </si>
+  <si>
+    <t>line</t>
+  </si>
+  <si>
+    <t>email</t>
+  </si>
+  <si>
+    <t>whatsapp</t>
+  </si>
+  <si>
+    <t>Index</t>
+  </si>
+  <si>
+    <t>0</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>3</t>
+  </si>
+  <si>
+    <t>4</t>
+  </si>
+  <si>
+    <t>Tab Name</t>
+  </si>
+  <si>
+    <t>5</t>
+  </si>
+  <si>
+    <t>6</t>
+  </si>
+  <si>
+    <t>All</t>
+  </si>
+  <si>
+    <t>Clip</t>
+  </si>
+  <si>
+    <t>Photo</t>
+  </si>
+  <si>
+    <t>Entertainment</t>
+  </si>
+  <si>
+    <t>News</t>
+  </si>
+  <si>
+    <t>Bloopers</t>
+  </si>
+  <si>
+    <t>Behind The Scenes</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="0;[Red]0"/>
+  </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -240,7 +363,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
@@ -252,6 +375,10 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -593,6 +720,58 @@
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
+      <selection sqref="A1:D2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="23.26953125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.90625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.1796875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.26953125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A1" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A2" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B2" t="s">
+        <v>36</v>
+      </c>
+      <c r="C2" t="s">
+        <v>41</v>
+      </c>
+      <c r="D2" t="s">
+        <v>42</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
       <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
@@ -640,11 +819,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
@@ -692,7 +871,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D3"/>
   <sheetViews>
@@ -755,7 +934,394 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:A3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1" s="7" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>51</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:E1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="2" max="2" width="20.81640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="23.54296875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A1" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>57</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D2" t="s">
+        <v>56</v>
+      </c>
+      <c r="E2" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>58</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D3" t="s">
+        <v>56</v>
+      </c>
+      <c r="E3" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>59</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C4" t="s">
+        <v>3</v>
+      </c>
+      <c r="D4" t="s">
+        <v>56</v>
+      </c>
+      <c r="E4" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>60</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C5" t="s">
+        <v>3</v>
+      </c>
+      <c r="D5" t="s">
+        <v>56</v>
+      </c>
+      <c r="E5" t="s">
+        <v>54</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B2" r:id="rId1"/>
+    <hyperlink ref="B3" r:id="rId2"/>
+    <hyperlink ref="B4" r:id="rId3"/>
+    <hyperlink ref="B5" r:id="rId4"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:B1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="20.81640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A1" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:B1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="17.6328125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="37.6328125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A1" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>61</v>
+      </c>
+      <c r="B2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A3" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="B3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A4" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="B4" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A5" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="B5" t="s">
+        <v>12</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A4" r:id="rId1"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H5" sqref="H5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="2" max="2" width="16.36328125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A1" s="10" t="s">
+        <v>71</v>
+      </c>
+      <c r="B1" s="10" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A2" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="B2" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A3" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="B3" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A4" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="B4" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A5" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="B5" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A6" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="B6" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A7" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="B7" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A8" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="B8" t="s">
+        <v>86</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A1" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A2" s="8" t="s">
+        <v>72</v>
+      </c>
+      <c r="B2" s="9" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A3" s="8" t="s">
+        <v>73</v>
+      </c>
+      <c r="B3" s="9" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A4" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="B4" s="9" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A5" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="B5" s="9" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A6" s="8" t="s">
+        <v>76</v>
+      </c>
+      <c r="B6" s="9" t="s">
+        <v>70</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C3"/>
   <sheetViews>
@@ -765,6 +1331,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
+    <col min="1" max="1" width="13.90625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.26953125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="37.6328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -806,7 +1374,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C3"/>
   <sheetViews>
@@ -860,7 +1428,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet3"/>
   <dimension ref="A1:C3"/>
@@ -917,7 +1485,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet4"/>
   <dimension ref="A1:C4"/>
@@ -980,7 +1548,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet5"/>
   <dimension ref="A1:B5"/>
@@ -1040,7 +1608,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D3"/>
   <sheetViews>
@@ -1106,7 +1674,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D2"/>
   <sheetViews>
@@ -1156,56 +1724,4 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:D2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <cols>
-    <col min="1" max="1" width="23.26953125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.90625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.1796875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="19.26953125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A1" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="B1" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="D1" s="4" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A2" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="B2" t="s">
-        <v>36</v>
-      </c>
-      <c r="C2" t="s">
-        <v>41</v>
-      </c>
-      <c r="D2" t="s">
-        <v>42</v>
-      </c>
-    </row>
-  </sheetData>
-  <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1"/>
-  </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
gti push update testcases chat and news add kanal
</commit_message>
<xml_diff>
--- a/src/main/java/data/data_test.xlsx
+++ b/src/main/java/data/data_test.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7450" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7450" firstSheet="16" activeTab="18"/>
   </bookViews>
   <sheets>
     <sheet name="Login_Success" sheetId="15" r:id="rId1"/>
@@ -30,6 +30,7 @@
     <sheet name="Mylist" sheetId="30" r:id="rId16"/>
     <sheet name="Forget_Password_Alert" sheetId="31" r:id="rId17"/>
     <sheet name="List_Tab_Menu_Exclusive" sheetId="34" r:id="rId18"/>
+    <sheet name="News_Default_Kanal" sheetId="36" r:id="rId19"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -41,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="91">
   <si>
     <t>Username</t>
   </si>
@@ -302,6 +303,18 @@
   </si>
   <si>
     <t>Behind The Scenes</t>
+  </si>
+  <si>
+    <t>Value</t>
+  </si>
+  <si>
+    <t>Berita Utama</t>
+  </si>
+  <si>
+    <t>Terkini</t>
+  </si>
+  <si>
+    <t>Populer</t>
   </si>
 </sst>
 </file>
@@ -1258,11 +1271,62 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C1" sqref="C1:C1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="2" max="2" width="11.7265625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A1" s="10" t="s">
+        <v>71</v>
+      </c>
+      <c r="B1" s="10" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A2" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="B2" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A3" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="B3" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A4" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="B4" t="s">
+        <v>90</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Update Testcases Edit Profile
</commit_message>
<xml_diff>
--- a/src/main/java/data/data_test.xlsx
+++ b/src/main/java/data/data_test.xlsx
@@ -9,28 +9,32 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7450" firstSheet="16" activeTab="18"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7450" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Login_Success" sheetId="15" r:id="rId1"/>
-    <sheet name="List_Share" sheetId="35" r:id="rId2"/>
-    <sheet name="Login_Alert_Username" sheetId="20" r:id="rId3"/>
-    <sheet name="Login_Alert_Password" sheetId="21" r:id="rId4"/>
-    <sheet name="Login_Alert_Popup" sheetId="16" r:id="rId5"/>
-    <sheet name="List_Menu_Account_Popup_Login" sheetId="12" r:id="rId6"/>
-    <sheet name="List_Menu_Account_Direct" sheetId="11" r:id="rId7"/>
-    <sheet name="Register_Email_Alert" sheetId="22" r:id="rId8"/>
-    <sheet name="Register_Password1_Alert_Email" sheetId="23" r:id="rId9"/>
-    <sheet name="Register_Password2_Alert_Email" sheetId="24" r:id="rId10"/>
-    <sheet name="Register_Password2_Alert_Phone" sheetId="26" r:id="rId11"/>
-    <sheet name="Register_Password1_Alert_Phone" sheetId="27" r:id="rId12"/>
-    <sheet name="Register_Phone_Alert" sheetId="25" r:id="rId13"/>
-    <sheet name="Register_List_Gender" sheetId="28" r:id="rId14"/>
-    <sheet name="Chat" sheetId="29" r:id="rId15"/>
-    <sheet name="Mylist" sheetId="30" r:id="rId16"/>
-    <sheet name="Forget_Password_Alert" sheetId="31" r:id="rId17"/>
-    <sheet name="List_Tab_Menu_Exclusive" sheetId="34" r:id="rId18"/>
-    <sheet name="News_Default_Kanal" sheetId="36" r:id="rId19"/>
+    <sheet name="Edit_Profile_Input" sheetId="38" r:id="rId2"/>
+    <sheet name="Edit_Profile_Alert_Named" sheetId="40" r:id="rId3"/>
+    <sheet name="Edit_Profile_Validate_Button" sheetId="44" r:id="rId4"/>
+    <sheet name="Edit_Profile_Alert_Phone" sheetId="41" r:id="rId5"/>
+    <sheet name="List_Share" sheetId="35" r:id="rId6"/>
+    <sheet name="Login_Alert_Username" sheetId="20" r:id="rId7"/>
+    <sheet name="Login_Alert_Password" sheetId="21" r:id="rId8"/>
+    <sheet name="Login_Alert_Popup" sheetId="16" r:id="rId9"/>
+    <sheet name="List_Menu_Account_Popup_Login" sheetId="12" r:id="rId10"/>
+    <sheet name="List_Menu_Account_Direct" sheetId="11" r:id="rId11"/>
+    <sheet name="Register_Email_Alert" sheetId="22" r:id="rId12"/>
+    <sheet name="Register_Password1_Alert_Email" sheetId="23" r:id="rId13"/>
+    <sheet name="Register_Password2_Alert_Email" sheetId="24" r:id="rId14"/>
+    <sheet name="Register_Password2_Alert_Phone" sheetId="26" r:id="rId15"/>
+    <sheet name="Register_Password1_Alert_Phone" sheetId="27" r:id="rId16"/>
+    <sheet name="Register_Phone_Alert" sheetId="25" r:id="rId17"/>
+    <sheet name="Register_List_Gender" sheetId="28" r:id="rId18"/>
+    <sheet name="Chat" sheetId="29" r:id="rId19"/>
+    <sheet name="Mylist" sheetId="30" r:id="rId20"/>
+    <sheet name="Forget_Password_Alert" sheetId="31" r:id="rId21"/>
+    <sheet name="List_Tab_Menu_Exclusive" sheetId="34" r:id="rId22"/>
+    <sheet name="News_Default_Kanal" sheetId="36" r:id="rId23"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -42,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="242" uniqueCount="99">
   <si>
     <t>Username</t>
   </si>
@@ -315,6 +319,30 @@
   </si>
   <si>
     <t>Populer</t>
+  </si>
+  <si>
+    <t>Edit</t>
+  </si>
+  <si>
+    <t>fullname</t>
+  </si>
+  <si>
+    <t>Input Edit</t>
+  </si>
+  <si>
+    <t>paijo@mailinator.com</t>
+  </si>
+  <si>
+    <t>myfullnameqcedit</t>
+  </si>
+  <si>
+    <t>nickname</t>
+  </si>
+  <si>
+    <t>Your Nickname Has Been Taken</t>
+  </si>
+  <si>
+    <t>phone-number</t>
   </si>
 </sst>
 </file>
@@ -677,7 +705,7 @@
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -729,6 +757,247 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr codeName="Sheet4"/>
+  <dimension ref="A1:C4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:C1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="2" max="3" width="11.81640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A1" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A2" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A3" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="29" x14ac:dyDescent="0.35">
+      <c r="A4" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>21</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr codeName="Sheet5"/>
+  <dimension ref="A1:B5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:B1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="12.1796875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.1796875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A1" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>26</v>
+      </c>
+      <c r="B3" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>27</v>
+      </c>
+      <c r="B4" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>28</v>
+      </c>
+      <c r="B5" t="s">
+        <v>32</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G2" sqref="G2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="20.81640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.90625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.453125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="32.81640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A1" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" t="s">
+        <v>36</v>
+      </c>
+      <c r="C2" t="s">
+        <v>36</v>
+      </c>
+      <c r="D2" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>35</v>
+      </c>
+      <c r="B3" t="s">
+        <v>36</v>
+      </c>
+      <c r="C3" t="s">
+        <v>36</v>
+      </c>
+      <c r="D3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:D2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="23.26953125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.90625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.453125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="30.90625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A1" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A2" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B2" t="s">
+        <v>39</v>
+      </c>
+      <c r="C2" t="s">
+        <v>39</v>
+      </c>
+      <c r="D2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D2"/>
   <sheetViews>
@@ -780,7 +1049,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D2"/>
   <sheetViews>
@@ -832,7 +1101,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D2"/>
   <sheetViews>
@@ -884,7 +1153,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D3"/>
   <sheetViews>
@@ -947,7 +1216,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A3"/>
   <sheetViews>
@@ -977,7 +1246,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E5"/>
   <sheetViews>
@@ -1088,7 +1357,59 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:D2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="19.54296875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.90625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.1796875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.90625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A1" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A2" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="B2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" t="s">
+        <v>92</v>
+      </c>
+      <c r="D2" t="s">
+        <v>95</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B2"/>
   <sheetViews>
@@ -1126,7 +1447,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B5"/>
   <sheetViews>
@@ -1189,7 +1510,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B8"/>
   <sheetViews>
@@ -1271,12 +1592,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1:C1048576"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1322,7 +1643,231 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:C2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="19.54296875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.90625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.81640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20.81640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="32.81640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A1" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A2" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="B2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" t="s">
+        <v>96</v>
+      </c>
+      <c r="D2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E2" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A3" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="B3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3" t="s">
+        <v>69</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E3" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A4" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="B4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C4" t="s">
+        <v>69</v>
+      </c>
+      <c r="D4" t="s">
+        <v>61</v>
+      </c>
+      <c r="E4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1"/>
+    <hyperlink ref="A3" r:id="rId2"/>
+    <hyperlink ref="D3" r:id="rId3"/>
+    <hyperlink ref="A4" r:id="rId4"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I14" sqref="I14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="19.54296875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.90625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.81640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A1" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A2" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="B2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A3" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="B3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A4" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="B4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C4" t="s">
+        <v>69</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1"/>
+    <hyperlink ref="A3" r:id="rId2"/>
+    <hyperlink ref="A4" r:id="rId3"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="19.54296875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.90625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.54296875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.81640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="33.7265625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A1" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A2" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="B2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" t="s">
+        <v>98</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="E2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B6"/>
   <sheetViews>
@@ -1385,7 +1930,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C3"/>
   <sheetViews>
@@ -1438,7 +1983,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C3"/>
   <sheetViews>
@@ -1492,7 +2037,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet3"/>
   <dimension ref="A1:C3"/>
@@ -1547,245 +2092,4 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr codeName="Sheet4"/>
-  <dimension ref="A1:C4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:C1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <cols>
-    <col min="2" max="3" width="11.81640625" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A1" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="B1" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="C1" s="4" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A2" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="B2" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="C2" s="5" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A3" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="B3" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="C3" s="5" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" ht="29" x14ac:dyDescent="0.35">
-      <c r="A4" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="B4" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="C4" s="5" t="s">
-        <v>21</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr codeName="Sheet5"/>
-  <dimension ref="A1:B5"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:B1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <cols>
-    <col min="1" max="1" width="12.1796875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="19.1796875" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A1" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="B1" s="4" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
-        <v>25</v>
-      </c>
-      <c r="B2" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
-        <v>26</v>
-      </c>
-      <c r="B3" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A4" t="s">
-        <v>27</v>
-      </c>
-      <c r="B4" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A5" t="s">
-        <v>28</v>
-      </c>
-      <c r="B5" t="s">
-        <v>32</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D3"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <cols>
-    <col min="1" max="1" width="20.81640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.90625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.453125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="32.81640625" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A1" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="B1" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="D1" s="4" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A2" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2" t="s">
-        <v>36</v>
-      </c>
-      <c r="C2" t="s">
-        <v>36</v>
-      </c>
-      <c r="D2" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
-        <v>35</v>
-      </c>
-      <c r="B3" t="s">
-        <v>36</v>
-      </c>
-      <c r="C3" t="s">
-        <v>36</v>
-      </c>
-      <c r="D3" t="s">
-        <v>9</v>
-      </c>
-    </row>
-  </sheetData>
-  <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1"/>
-  </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:D2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <cols>
-    <col min="1" max="1" width="23.26953125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.90625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.453125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="30.90625" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A1" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="B1" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="D1" s="4" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A2" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="B2" t="s">
-        <v>39</v>
-      </c>
-      <c r="C2" t="s">
-        <v>39</v>
-      </c>
-      <c r="D2" t="s">
-        <v>40</v>
-      </c>
-    </row>
-  </sheetData>
-  <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1"/>
-  </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
Set selenium grid to local
</commit_message>
<xml_diff>
--- a/src/main/java/data/data_test.xlsx
+++ b/src/main/java/data/data_test.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7450" firstSheet="6" activeTab="8"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7450" firstSheet="2" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Login_Success" sheetId="15" r:id="rId1"/>
@@ -51,7 +51,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="297" uniqueCount="119">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="302" uniqueCount="119">
   <si>
     <t>Username</t>
   </si>
@@ -2161,55 +2161,16 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A5"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A1" s="10" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A4" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A5" t="s">
-        <v>102</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:B4"/>
+  <dimension ref="A1:B5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="5.453125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.81640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.35">
@@ -2217,7 +2178,7 @@
         <v>71</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>103</v>
+        <v>52</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">
@@ -2225,7 +2186,7 @@
         <v>72</v>
       </c>
       <c r="B2" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
@@ -2233,7 +2194,7 @@
         <v>73</v>
       </c>
       <c r="B3" t="s">
-        <v>84</v>
+        <v>100</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.35">
@@ -2241,7 +2202,15 @@
         <v>74</v>
       </c>
       <c r="B4" t="s">
-        <v>105</v>
+        <v>101</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A5" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="B5" t="s">
+        <v>102</v>
       </c>
     </row>
   </sheetData>
@@ -2250,16 +2219,17 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B6"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:B6"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <cols>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:B4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="5.453125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="9.81640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -2276,7 +2246,7 @@
         <v>72</v>
       </c>
       <c r="B2" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
@@ -2284,7 +2254,7 @@
         <v>73</v>
       </c>
       <c r="B3" t="s">
-        <v>107</v>
+        <v>84</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.35">
@@ -2292,6 +2262,57 @@
         <v>74</v>
       </c>
       <c r="B4" t="s">
+        <v>105</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:B6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="2" max="2" width="9.81640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A1" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A2" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="B2" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A3" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="B3" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A4" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="B4" t="s">
         <v>52</v>
       </c>
     </row>
@@ -2406,7 +2427,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
update testcase live event and sticky ads
</commit_message>
<xml_diff>
--- a/src/main/java/data/data_test.xlsx
+++ b/src/main/java/data/data_test.xlsx
@@ -9,39 +9,40 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7450" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7450" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Login_Success" sheetId="15" r:id="rId1"/>
     <sheet name="Continue_Watching" sheetId="51" r:id="rId2"/>
-    <sheet name="Edit_Profile_Input" sheetId="38" r:id="rId3"/>
-    <sheet name="Edit_Profile_Alert_Named" sheetId="40" r:id="rId4"/>
-    <sheet name="Edit_Profile_Validate_Button" sheetId="44" r:id="rId5"/>
-    <sheet name="Live_Tv_Active_Tab" sheetId="45" r:id="rId6"/>
-    <sheet name="Live_Tv_Tab_Live_And_Catch" sheetId="50" r:id="rId7"/>
-    <sheet name="Homepage_Menu_Tengah" sheetId="46" r:id="rId8"/>
-    <sheet name="Homepage_Menu_Bawah" sheetId="47" r:id="rId9"/>
-    <sheet name="Homepage_Menu_Bawah_Direct" sheetId="48" r:id="rId10"/>
-    <sheet name="Homepage_Menu_Tengah_Direct" sheetId="49" r:id="rId11"/>
-    <sheet name="Edit_Profile_Alert_Phone" sheetId="41" r:id="rId12"/>
-    <sheet name="List_Share" sheetId="35" r:id="rId13"/>
-    <sheet name="Login_Alert_Username" sheetId="20" r:id="rId14"/>
-    <sheet name="Login_Alert_Password" sheetId="21" r:id="rId15"/>
-    <sheet name="Login_Alert_Popup" sheetId="16" r:id="rId16"/>
-    <sheet name="List_Menu_Account_Popup_Login" sheetId="12" r:id="rId17"/>
-    <sheet name="List_Menu_Account_Direct" sheetId="11" r:id="rId18"/>
-    <sheet name="Register_Email_Alert" sheetId="22" r:id="rId19"/>
-    <sheet name="Register_Password1_Alert_Email" sheetId="23" r:id="rId20"/>
-    <sheet name="Register_Password2_Alert_Email" sheetId="24" r:id="rId21"/>
-    <sheet name="Register_Password2_Alert_Phone" sheetId="26" r:id="rId22"/>
-    <sheet name="Register_Password1_Alert_Phone" sheetId="27" r:id="rId23"/>
-    <sheet name="Register_Phone_Alert" sheetId="25" r:id="rId24"/>
-    <sheet name="Register_List_Gender" sheetId="28" r:id="rId25"/>
-    <sheet name="Chat" sheetId="29" r:id="rId26"/>
-    <sheet name="Mylist" sheetId="30" r:id="rId27"/>
-    <sheet name="Forget_Password_Alert" sheetId="31" r:id="rId28"/>
-    <sheet name="List_Tab_Menu_Exclusive" sheetId="34" r:id="rId29"/>
-    <sheet name="News_Default_Kanal" sheetId="36" r:id="rId30"/>
+    <sheet name="List_Tab_Live_Event" sheetId="52" r:id="rId3"/>
+    <sheet name="Edit_Profile_Input" sheetId="38" r:id="rId4"/>
+    <sheet name="Edit_Profile_Alert_Named" sheetId="40" r:id="rId5"/>
+    <sheet name="Edit_Profile_Validate_Button" sheetId="44" r:id="rId6"/>
+    <sheet name="Live_Tv_Active_Tab" sheetId="45" r:id="rId7"/>
+    <sheet name="Live_Tv_Tab_Live_And_Catch" sheetId="50" r:id="rId8"/>
+    <sheet name="Homepage_Menu_Tengah" sheetId="46" r:id="rId9"/>
+    <sheet name="Homepage_Menu_Bawah" sheetId="47" r:id="rId10"/>
+    <sheet name="Homepage_Menu_Bawah_Direct" sheetId="48" r:id="rId11"/>
+    <sheet name="Homepage_Menu_Tengah_Direct" sheetId="49" r:id="rId12"/>
+    <sheet name="Edit_Profile_Alert_Phone" sheetId="41" r:id="rId13"/>
+    <sheet name="List_Share" sheetId="35" r:id="rId14"/>
+    <sheet name="Login_Alert_Username" sheetId="20" r:id="rId15"/>
+    <sheet name="Login_Alert_Password" sheetId="21" r:id="rId16"/>
+    <sheet name="Login_Alert_Popup" sheetId="16" r:id="rId17"/>
+    <sheet name="List_Menu_Account_Popup_Login" sheetId="12" r:id="rId18"/>
+    <sheet name="List_Menu_Account_Direct" sheetId="11" r:id="rId19"/>
+    <sheet name="Register_Email_Alert" sheetId="22" r:id="rId20"/>
+    <sheet name="Register_Password1_Alert_Email" sheetId="23" r:id="rId21"/>
+    <sheet name="Register_Password2_Alert_Email" sheetId="24" r:id="rId22"/>
+    <sheet name="Register_Password2_Alert_Phone" sheetId="26" r:id="rId23"/>
+    <sheet name="Register_Password1_Alert_Phone" sheetId="27" r:id="rId24"/>
+    <sheet name="Register_Phone_Alert" sheetId="25" r:id="rId25"/>
+    <sheet name="Register_List_Gender" sheetId="28" r:id="rId26"/>
+    <sheet name="Chat" sheetId="29" r:id="rId27"/>
+    <sheet name="Mylist" sheetId="30" r:id="rId28"/>
+    <sheet name="Forget_Password_Alert" sheetId="31" r:id="rId29"/>
+    <sheet name="List_Tab_Menu_Exclusive" sheetId="34" r:id="rId30"/>
+    <sheet name="News_Default_Kanal" sheetId="36" r:id="rId31"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -53,7 +54,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="312" uniqueCount="121">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="318" uniqueCount="123">
   <si>
     <t>Username</t>
   </si>
@@ -416,6 +417,12 @@
   </si>
   <si>
     <t>Live</t>
+  </si>
+  <si>
+    <t>Tabs</t>
+  </si>
+  <si>
+    <t>Missed Event</t>
   </si>
 </sst>
 </file>
@@ -831,6 +838,72 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:B6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="2" max="2" width="9.81640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A1" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A2" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="B2" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A3" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="B3" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A4" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="B4" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A5" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="B5" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A6" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="B6" t="s">
+        <v>109</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -915,7 +988,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C4"/>
   <sheetViews>
@@ -979,7 +1052,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E2"/>
   <sheetViews>
@@ -1038,7 +1111,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B6"/>
   <sheetViews>
@@ -1101,7 +1174,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C3"/>
   <sheetViews>
@@ -1154,7 +1227,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C3"/>
   <sheetViews>
@@ -1208,7 +1281,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet3"/>
   <dimension ref="A1:C3"/>
@@ -1265,7 +1338,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet4"/>
   <dimension ref="A1:C4"/>
@@ -1328,7 +1401,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet5"/>
   <dimension ref="A1:B5"/>
@@ -1388,7 +1461,45 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="20.81640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.90625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D3"/>
   <sheetViews>
@@ -1454,45 +1565,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B2"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <cols>
-    <col min="1" max="1" width="20.81640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.90625" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A1" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="3" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A2" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-  </sheetData>
-  <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1"/>
-  </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D2"/>
   <sheetViews>
@@ -1544,7 +1617,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D2"/>
   <sheetViews>
@@ -1596,7 +1669,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D2"/>
   <sheetViews>
@@ -1648,7 +1721,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D2"/>
   <sheetViews>
@@ -1700,7 +1773,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D3"/>
   <sheetViews>
@@ -1763,7 +1836,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A3"/>
   <sheetViews>
@@ -1793,7 +1866,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E5"/>
   <sheetViews>
@@ -1904,7 +1977,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B2"/>
   <sheetViews>
@@ -1942,7 +2015,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B5"/>
   <sheetViews>
@@ -2005,7 +2078,50 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E12" sqref="E12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="2" max="2" width="11.81640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A1" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A2" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="B2" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A3" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="B3" t="s">
+        <v>122</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet30.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B8"/>
   <sheetViews>
@@ -2087,7 +2203,58 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet31.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="2" max="2" width="11.7265625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A1" s="10" t="s">
+        <v>71</v>
+      </c>
+      <c r="B1" s="10" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A2" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="B2" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A3" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="B3" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A4" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="B4" t="s">
+        <v>90</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D2"/>
   <sheetViews>
@@ -2139,58 +2306,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet30.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <cols>
-    <col min="2" max="2" width="11.7265625" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A1" s="10" t="s">
-        <v>71</v>
-      </c>
-      <c r="B1" s="10" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A2" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="B2" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A3" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="B3" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A4" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="B4" t="s">
-        <v>90</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E4"/>
   <sheetViews>
@@ -2286,7 +2402,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C4"/>
   <sheetViews>
@@ -2355,7 +2471,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B5"/>
   <sheetViews>
@@ -2415,7 +2531,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B3"/>
   <sheetViews>
@@ -2459,7 +2575,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B4"/>
   <sheetViews>
@@ -2509,70 +2625,4 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B6"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:B6"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <cols>
-    <col min="2" max="2" width="9.81640625" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A1" s="4" t="s">
-        <v>71</v>
-      </c>
-      <c r="B1" s="4" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A2" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="B2" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A3" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="B3" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A4" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="B4" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A5" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="B5" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A6" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="B6" t="s">
-        <v>109</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
update thread sleep Testcases
</commit_message>
<xml_diff>
--- a/src/main/java/data/data_test.xlsx
+++ b/src/main/java/data/data_test.xlsx
@@ -9,40 +9,41 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7450" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7450" firstSheet="1" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Login_Success" sheetId="15" r:id="rId1"/>
     <sheet name="Continue_Watching" sheetId="51" r:id="rId2"/>
     <sheet name="List_Tab_Live_Event" sheetId="52" r:id="rId3"/>
-    <sheet name="Edit_Profile_Input" sheetId="38" r:id="rId4"/>
-    <sheet name="Edit_Profile_Alert_Named" sheetId="40" r:id="rId5"/>
-    <sheet name="Edit_Profile_Validate_Button" sheetId="44" r:id="rId6"/>
-    <sheet name="Live_Tv_Active_Tab" sheetId="45" r:id="rId7"/>
-    <sheet name="Live_Tv_Tab_Live_And_Catch" sheetId="50" r:id="rId8"/>
-    <sheet name="Homepage_Menu_Tengah" sheetId="46" r:id="rId9"/>
-    <sheet name="Homepage_Menu_Bawah" sheetId="47" r:id="rId10"/>
-    <sheet name="Homepage_Menu_Bawah_Direct" sheetId="48" r:id="rId11"/>
-    <sheet name="Homepage_Menu_Tengah_Direct" sheetId="49" r:id="rId12"/>
-    <sheet name="Edit_Profile_Alert_Phone" sheetId="41" r:id="rId13"/>
-    <sheet name="List_Share" sheetId="35" r:id="rId14"/>
-    <sheet name="Login_Alert_Username" sheetId="20" r:id="rId15"/>
-    <sheet name="Login_Alert_Password" sheetId="21" r:id="rId16"/>
-    <sheet name="Login_Alert_Popup" sheetId="16" r:id="rId17"/>
-    <sheet name="List_Menu_Account_Popup_Login" sheetId="12" r:id="rId18"/>
-    <sheet name="List_Menu_Account_Direct" sheetId="11" r:id="rId19"/>
-    <sheet name="Register_Email_Alert" sheetId="22" r:id="rId20"/>
-    <sheet name="Register_Password1_Alert_Email" sheetId="23" r:id="rId21"/>
-    <sheet name="Register_Password2_Alert_Email" sheetId="24" r:id="rId22"/>
-    <sheet name="Register_Password2_Alert_Phone" sheetId="26" r:id="rId23"/>
-    <sheet name="Register_Password1_Alert_Phone" sheetId="27" r:id="rId24"/>
-    <sheet name="Register_Phone_Alert" sheetId="25" r:id="rId25"/>
-    <sheet name="Register_List_Gender" sheetId="28" r:id="rId26"/>
-    <sheet name="Chat" sheetId="29" r:id="rId27"/>
-    <sheet name="Mylist" sheetId="30" r:id="rId28"/>
-    <sheet name="Forget_Password_Alert" sheetId="31" r:id="rId29"/>
-    <sheet name="List_Tab_Menu_Exclusive" sheetId="34" r:id="rId30"/>
-    <sheet name="News_Default_Kanal" sheetId="36" r:id="rId31"/>
+    <sheet name="Phone_Code_Number" sheetId="53" r:id="rId4"/>
+    <sheet name="Edit_Profile_Input" sheetId="38" r:id="rId5"/>
+    <sheet name="Edit_Profile_Alert_Named" sheetId="40" r:id="rId6"/>
+    <sheet name="Edit_Profile_Validate_Button" sheetId="44" r:id="rId7"/>
+    <sheet name="Live_Tv_Active_Tab" sheetId="45" r:id="rId8"/>
+    <sheet name="Live_Tv_Tab_Live_And_Catch" sheetId="50" r:id="rId9"/>
+    <sheet name="Homepage_Menu_Tengah" sheetId="46" r:id="rId10"/>
+    <sheet name="Homepage_Menu_Bawah" sheetId="47" r:id="rId11"/>
+    <sheet name="Homepage_Menu_Bawah_Direct" sheetId="48" r:id="rId12"/>
+    <sheet name="Homepage_Menu_Tengah_Direct" sheetId="49" r:id="rId13"/>
+    <sheet name="Edit_Profile_Alert_Phone" sheetId="41" r:id="rId14"/>
+    <sheet name="List_Share" sheetId="35" r:id="rId15"/>
+    <sheet name="Login_Alert_Username" sheetId="20" r:id="rId16"/>
+    <sheet name="Login_Alert_Password" sheetId="21" r:id="rId17"/>
+    <sheet name="Login_Alert_Popup" sheetId="16" r:id="rId18"/>
+    <sheet name="List_Menu_Account_Popup_Login" sheetId="12" r:id="rId19"/>
+    <sheet name="List_Menu_Account_Direct" sheetId="11" r:id="rId20"/>
+    <sheet name="Register_Email_Alert" sheetId="22" r:id="rId21"/>
+    <sheet name="Register_Password1_Alert_Email" sheetId="23" r:id="rId22"/>
+    <sheet name="Register_Password2_Alert_Email" sheetId="24" r:id="rId23"/>
+    <sheet name="Register_Password2_Alert_Phone" sheetId="26" r:id="rId24"/>
+    <sheet name="Register_Password1_Alert_Phone" sheetId="27" r:id="rId25"/>
+    <sheet name="Register_Phone_Alert" sheetId="25" r:id="rId26"/>
+    <sheet name="Register_List_Gender" sheetId="28" r:id="rId27"/>
+    <sheet name="Chat" sheetId="29" r:id="rId28"/>
+    <sheet name="Mylist" sheetId="30" r:id="rId29"/>
+    <sheet name="Forget_Password_Alert" sheetId="31" r:id="rId30"/>
+    <sheet name="List_Tab_Menu_Exclusive" sheetId="34" r:id="rId31"/>
+    <sheet name="News_Default_Kanal" sheetId="36" r:id="rId32"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -54,7 +55,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="318" uniqueCount="123">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="324" uniqueCount="126">
   <si>
     <t>Username</t>
   </si>
@@ -423,6 +424,15 @@
   </si>
   <si>
     <t>Missed Event</t>
+  </si>
+  <si>
+    <t>8227884</t>
+  </si>
+  <si>
+    <t>Country Code</t>
+  </si>
+  <si>
+    <t>AI</t>
   </si>
 </sst>
 </file>
@@ -838,14 +848,15 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B6"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:B6"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <cols>
+  <dimension ref="A1:B4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:B4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="5.453125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="9.81640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -862,7 +873,7 @@
         <v>72</v>
       </c>
       <c r="B2" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
@@ -870,7 +881,7 @@
         <v>73</v>
       </c>
       <c r="B3" t="s">
-        <v>107</v>
+        <v>84</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.35">
@@ -878,6 +889,57 @@
         <v>74</v>
       </c>
       <c r="B4" t="s">
+        <v>105</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:B6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="2" max="2" width="9.81640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A1" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A2" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="B2" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A3" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="B3" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A4" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="B4" t="s">
         <v>52</v>
       </c>
     </row>
@@ -902,7 +964,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C6"/>
   <sheetViews>
@@ -988,7 +1050,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C4"/>
   <sheetViews>
@@ -1052,7 +1114,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E2"/>
   <sheetViews>
@@ -1111,7 +1173,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B6"/>
   <sheetViews>
@@ -1174,7 +1236,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C3"/>
   <sheetViews>
@@ -1227,7 +1289,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C3"/>
   <sheetViews>
@@ -1281,7 +1343,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet3"/>
   <dimension ref="A1:C3"/>
@@ -1338,7 +1400,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet4"/>
   <dimension ref="A1:C4"/>
@@ -1401,7 +1463,45 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="20.81640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.90625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet5"/>
   <dimension ref="A1:B5"/>
@@ -1461,45 +1561,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <cols>
-    <col min="1" max="1" width="20.81640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.90625" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A1" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="3" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A2" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-  </sheetData>
-  <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1"/>
-  </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D3"/>
   <sheetViews>
@@ -1565,7 +1627,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D2"/>
   <sheetViews>
@@ -1617,7 +1679,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D2"/>
   <sheetViews>
@@ -1669,7 +1731,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D2"/>
   <sheetViews>
@@ -1721,7 +1783,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D2"/>
   <sheetViews>
@@ -1773,7 +1835,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D3"/>
   <sheetViews>
@@ -1836,7 +1898,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A3"/>
   <sheetViews>
@@ -1866,7 +1928,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E5"/>
   <sheetViews>
@@ -1977,7 +2039,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B2"/>
   <sheetViews>
@@ -2015,7 +2077,50 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I2" sqref="I2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="2" max="2" width="11.81640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A1" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A2" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="B2" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A3" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="B3" t="s">
+        <v>122</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet30.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B5"/>
   <sheetViews>
@@ -2078,25 +2183,25 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B3"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <cols>
-    <col min="2" max="2" width="11.81640625" bestFit="1" customWidth="1"/>
+<file path=xl/worksheets/sheet31.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H5" sqref="H5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="2" max="2" width="16.36328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="10" t="s">
         <v>71</v>
       </c>
-      <c r="B1" s="4" t="s">
-        <v>121</v>
+      <c r="B1" s="10" t="s">
+        <v>77</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">
@@ -2104,7 +2209,7 @@
         <v>72</v>
       </c>
       <c r="B2" t="s">
-        <v>107</v>
+        <v>80</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
@@ -2112,26 +2217,65 @@
         <v>73</v>
       </c>
       <c r="B3" t="s">
-        <v>122</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet30.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B8"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H5" sqref="H5"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <cols>
-    <col min="2" max="2" width="16.36328125" bestFit="1" customWidth="1"/>
+        <v>81</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A4" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="B4" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A5" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="B5" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A6" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="B6" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A7" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="B7" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A8" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="B8" t="s">
+        <v>86</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet32.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="2" max="2" width="11.7265625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.35">
@@ -2139,7 +2283,7 @@
         <v>71</v>
       </c>
       <c r="B1" s="10" t="s">
-        <v>77</v>
+        <v>87</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">
@@ -2147,7 +2291,7 @@
         <v>72</v>
       </c>
       <c r="B2" t="s">
-        <v>80</v>
+        <v>88</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
@@ -2155,7 +2299,7 @@
         <v>73</v>
       </c>
       <c r="B3" t="s">
-        <v>81</v>
+        <v>89</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.35">
@@ -2163,89 +2307,48 @@
         <v>74</v>
       </c>
       <c r="B4" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A5" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="B5" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A6" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="B6" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A7" s="2" t="s">
+        <v>90</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="3" max="3" width="12.26953125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A1" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A2" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="B7" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A8" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="B8" t="s">
-        <v>86</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet31.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <cols>
-    <col min="2" max="2" width="11.7265625" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A1" s="10" t="s">
-        <v>71</v>
-      </c>
-      <c r="B1" s="10" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A2" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="B2" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A3" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="B3" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A4" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="B4" t="s">
-        <v>90</v>
+      <c r="C2" t="s">
+        <v>125</v>
       </c>
     </row>
   </sheetData>
@@ -2254,7 +2357,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D2"/>
   <sheetViews>
@@ -2306,7 +2409,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E4"/>
   <sheetViews>
@@ -2402,7 +2505,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C4"/>
   <sheetViews>
@@ -2471,7 +2574,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B5"/>
   <sheetViews>
@@ -2531,7 +2634,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B3"/>
   <sheetViews>
@@ -2573,56 +2676,4 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:B4"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <cols>
-    <col min="1" max="1" width="5.453125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.81640625" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A1" s="4" t="s">
-        <v>71</v>
-      </c>
-      <c r="B1" s="4" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A2" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="B2" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A3" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="B3" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A4" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="B4" t="s">
-        <v>105</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
update testcases phone code
</commit_message>
<xml_diff>
--- a/src/main/java/data/data_test.xlsx
+++ b/src/main/java/data/data_test.xlsx
@@ -9,41 +9,43 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7450" firstSheet="1" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7450" firstSheet="1" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Login_Success" sheetId="15" r:id="rId1"/>
     <sheet name="Continue_Watching" sheetId="51" r:id="rId2"/>
     <sheet name="List_Tab_Live_Event" sheetId="52" r:id="rId3"/>
     <sheet name="Phone_Code_Number" sheetId="53" r:id="rId4"/>
-    <sheet name="Edit_Profile_Input" sheetId="38" r:id="rId5"/>
-    <sheet name="Edit_Profile_Alert_Named" sheetId="40" r:id="rId6"/>
-    <sheet name="Edit_Profile_Validate_Button" sheetId="44" r:id="rId7"/>
-    <sheet name="Live_Tv_Active_Tab" sheetId="45" r:id="rId8"/>
-    <sheet name="Live_Tv_Tab_Live_And_Catch" sheetId="50" r:id="rId9"/>
-    <sheet name="Homepage_Menu_Tengah" sheetId="46" r:id="rId10"/>
-    <sheet name="Homepage_Menu_Bawah" sheetId="47" r:id="rId11"/>
-    <sheet name="Homepage_Menu_Bawah_Direct" sheetId="48" r:id="rId12"/>
-    <sheet name="Homepage_Menu_Tengah_Direct" sheetId="49" r:id="rId13"/>
-    <sheet name="Edit_Profile_Alert_Phone" sheetId="41" r:id="rId14"/>
-    <sheet name="List_Share" sheetId="35" r:id="rId15"/>
-    <sheet name="Login_Alert_Username" sheetId="20" r:id="rId16"/>
-    <sheet name="Login_Alert_Password" sheetId="21" r:id="rId17"/>
-    <sheet name="Login_Alert_Popup" sheetId="16" r:id="rId18"/>
-    <sheet name="List_Menu_Account_Popup_Login" sheetId="12" r:id="rId19"/>
-    <sheet name="List_Menu_Account_Direct" sheetId="11" r:id="rId20"/>
-    <sheet name="Register_Email_Alert" sheetId="22" r:id="rId21"/>
-    <sheet name="Register_Password1_Alert_Email" sheetId="23" r:id="rId22"/>
-    <sheet name="Register_Password2_Alert_Email" sheetId="24" r:id="rId23"/>
-    <sheet name="Register_Password2_Alert_Phone" sheetId="26" r:id="rId24"/>
-    <sheet name="Register_Password1_Alert_Phone" sheetId="27" r:id="rId25"/>
-    <sheet name="Register_Phone_Alert" sheetId="25" r:id="rId26"/>
-    <sheet name="Register_List_Gender" sheetId="28" r:id="rId27"/>
-    <sheet name="Chat" sheetId="29" r:id="rId28"/>
-    <sheet name="Mylist" sheetId="30" r:id="rId29"/>
-    <sheet name="Forget_Password_Alert" sheetId="31" r:id="rId30"/>
-    <sheet name="List_Tab_Menu_Exclusive" sheetId="34" r:id="rId31"/>
-    <sheet name="News_Default_Kanal" sheetId="36" r:id="rId32"/>
+    <sheet name="Sheet1" sheetId="54" r:id="rId5"/>
+    <sheet name="Login_Phone_Code" sheetId="55" r:id="rId6"/>
+    <sheet name="Edit_Profile_Input" sheetId="38" r:id="rId7"/>
+    <sheet name="Edit_Profile_Alert_Named" sheetId="40" r:id="rId8"/>
+    <sheet name="Edit_Profile_Validate_Button" sheetId="44" r:id="rId9"/>
+    <sheet name="Live_Tv_Active_Tab" sheetId="45" r:id="rId10"/>
+    <sheet name="Live_Tv_Tab_Live_And_Catch" sheetId="50" r:id="rId11"/>
+    <sheet name="Homepage_Menu_Tengah" sheetId="46" r:id="rId12"/>
+    <sheet name="Homepage_Menu_Bawah" sheetId="47" r:id="rId13"/>
+    <sheet name="Homepage_Menu_Bawah_Direct" sheetId="48" r:id="rId14"/>
+    <sheet name="Homepage_Menu_Tengah_Direct" sheetId="49" r:id="rId15"/>
+    <sheet name="Edit_Profile_Alert_Phone" sheetId="41" r:id="rId16"/>
+    <sheet name="List_Share" sheetId="35" r:id="rId17"/>
+    <sheet name="Login_Alert_Username" sheetId="20" r:id="rId18"/>
+    <sheet name="Login_Alert_Password" sheetId="21" r:id="rId19"/>
+    <sheet name="Login_Alert_Popup" sheetId="16" r:id="rId20"/>
+    <sheet name="List_Menu_Account_Popup_Login" sheetId="12" r:id="rId21"/>
+    <sheet name="List_Menu_Account_Direct" sheetId="11" r:id="rId22"/>
+    <sheet name="Register_Email_Alert" sheetId="22" r:id="rId23"/>
+    <sheet name="Register_Password1_Alert_Email" sheetId="23" r:id="rId24"/>
+    <sheet name="Register_Password2_Alert_Email" sheetId="24" r:id="rId25"/>
+    <sheet name="Register_Password2_Alert_Phone" sheetId="26" r:id="rId26"/>
+    <sheet name="Register_Password1_Alert_Phone" sheetId="27" r:id="rId27"/>
+    <sheet name="Register_Phone_Alert" sheetId="25" r:id="rId28"/>
+    <sheet name="Register_List_Gender" sheetId="28" r:id="rId29"/>
+    <sheet name="Chat" sheetId="29" r:id="rId30"/>
+    <sheet name="Mylist" sheetId="30" r:id="rId31"/>
+    <sheet name="Forget_Password_Alert" sheetId="31" r:id="rId32"/>
+    <sheet name="List_Tab_Menu_Exclusive" sheetId="34" r:id="rId33"/>
+    <sheet name="News_Default_Kanal" sheetId="36" r:id="rId34"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -55,7 +57,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="324" uniqueCount="126">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="334" uniqueCount="133">
   <si>
     <t>Username</t>
   </si>
@@ -433,6 +435,27 @@
   </si>
   <si>
     <t>AI</t>
+  </si>
+  <si>
+    <t>Country</t>
+  </si>
+  <si>
+    <t>Display name</t>
+  </si>
+  <si>
+    <t>united states</t>
+  </si>
+  <si>
+    <t>dikaphonecod</t>
+  </si>
+  <si>
+    <t>2126712234</t>
+  </si>
+  <si>
+    <t>US</t>
+  </si>
+  <si>
+    <t>Country Name</t>
   </si>
 </sst>
 </file>
@@ -848,16 +871,16 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:B4"/>
+  <dimension ref="A1:B5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="5.453125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.81640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.35">
@@ -865,7 +888,7 @@
         <v>71</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>103</v>
+        <v>52</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">
@@ -873,7 +896,7 @@
         <v>72</v>
       </c>
       <c r="B2" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
@@ -881,7 +904,7 @@
         <v>73</v>
       </c>
       <c r="B3" t="s">
-        <v>84</v>
+        <v>100</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.35">
@@ -889,7 +912,15 @@
         <v>74</v>
       </c>
       <c r="B4" t="s">
-        <v>105</v>
+        <v>101</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A5" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="B5" t="s">
+        <v>102</v>
       </c>
     </row>
   </sheetData>
@@ -900,15 +931,16 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B6"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:B6"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <cols>
-    <col min="2" max="2" width="9.81640625" bestFit="1" customWidth="1"/>
+  <dimension ref="A1:B3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="5.453125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.81640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.35">
@@ -916,7 +948,7 @@
         <v>71</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>103</v>
+        <v>87</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">
@@ -924,7 +956,7 @@
         <v>72</v>
       </c>
       <c r="B2" t="s">
-        <v>106</v>
+        <v>120</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
@@ -932,7 +964,51 @@
         <v>73</v>
       </c>
       <c r="B3" t="s">
-        <v>107</v>
+        <v>119</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:B4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="5.453125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.81640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A1" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A2" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="B2" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A3" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="B3" t="s">
+        <v>84</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.35">
@@ -940,6 +1016,57 @@
         <v>74</v>
       </c>
       <c r="B4" t="s">
+        <v>105</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:B6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="2" max="2" width="9.81640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A1" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A2" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="B2" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A3" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="B3" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A4" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="B4" t="s">
         <v>52</v>
       </c>
     </row>
@@ -964,7 +1091,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C6"/>
   <sheetViews>
@@ -1050,7 +1177,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C4"/>
   <sheetViews>
@@ -1114,7 +1241,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E2"/>
   <sheetViews>
@@ -1173,7 +1300,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B6"/>
   <sheetViews>
@@ -1236,7 +1363,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C3"/>
   <sheetViews>
@@ -1289,7 +1416,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C3"/>
   <sheetViews>
@@ -1343,7 +1470,45 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="20.81640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.90625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet3"/>
   <dimension ref="A1:C3"/>
@@ -1400,7 +1565,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet4"/>
   <dimension ref="A1:C4"/>
@@ -1463,45 +1628,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <cols>
-    <col min="1" max="1" width="20.81640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.90625" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A1" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="3" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A2" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-  </sheetData>
-  <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1"/>
-  </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet5"/>
   <dimension ref="A1:B5"/>
@@ -1561,7 +1688,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D3"/>
   <sheetViews>
@@ -1627,7 +1754,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D2"/>
   <sheetViews>
@@ -1679,7 +1806,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D2"/>
   <sheetViews>
@@ -1731,7 +1858,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D2"/>
   <sheetViews>
@@ -1783,7 +1910,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D2"/>
   <sheetViews>
@@ -1835,7 +1962,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D3"/>
   <sheetViews>
@@ -1898,7 +2025,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A3"/>
   <sheetViews>
@@ -1928,7 +2055,50 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I2" sqref="I2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="2" max="2" width="11.81640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A1" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A2" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="B2" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A3" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="B3" t="s">
+        <v>122</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet30.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E5"/>
   <sheetViews>
@@ -2039,7 +2209,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet31.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B2"/>
   <sheetViews>
@@ -2077,25 +2247,88 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B3"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I2" sqref="I2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <cols>
-    <col min="2" max="2" width="11.81640625" bestFit="1" customWidth="1"/>
+<file path=xl/worksheets/sheet32.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:B1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="17.6328125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="37.6328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>61</v>
+      </c>
+      <c r="B2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A3" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="B3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A4" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="B4" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A5" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="B5" t="s">
+        <v>12</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A4" r:id="rId1"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet33.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H5" sqref="H5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="2" max="2" width="16.36328125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A1" s="10" t="s">
         <v>71</v>
       </c>
-      <c r="B1" s="4" t="s">
-        <v>121</v>
+      <c r="B1" s="10" t="s">
+        <v>77</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">
@@ -2103,7 +2336,7 @@
         <v>72</v>
       </c>
       <c r="B2" t="s">
-        <v>107</v>
+        <v>80</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
@@ -2111,89 +2344,65 @@
         <v>73</v>
       </c>
       <c r="B3" t="s">
-        <v>122</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet30.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B5"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:B1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <cols>
-    <col min="1" max="1" width="17.6328125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="37.6328125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A1" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="4" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
-        <v>61</v>
-      </c>
-      <c r="B2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A3" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="B3" t="s">
-        <v>14</v>
+        <v>81</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A4" s="1" t="s">
-        <v>64</v>
+      <c r="A4" s="2" t="s">
+        <v>74</v>
       </c>
       <c r="B4" t="s">
-        <v>12</v>
+        <v>82</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" s="2" t="s">
-        <v>63</v>
+        <v>75</v>
       </c>
       <c r="B5" t="s">
-        <v>12</v>
-      </c>
-    </row>
-  </sheetData>
-  <hyperlinks>
-    <hyperlink ref="A4" r:id="rId1"/>
-  </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet31.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B8"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H5" sqref="H5"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <cols>
-    <col min="2" max="2" width="16.36328125" bestFit="1" customWidth="1"/>
+        <v>83</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A6" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="B6" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A7" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="B7" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A8" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="B8" t="s">
+        <v>86</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet34.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="2" max="2" width="11.7265625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.35">
@@ -2201,7 +2410,7 @@
         <v>71</v>
       </c>
       <c r="B1" s="10" t="s">
-        <v>77</v>
+        <v>87</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">
@@ -2209,7 +2418,7 @@
         <v>72</v>
       </c>
       <c r="B2" t="s">
-        <v>80</v>
+        <v>88</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
@@ -2217,7 +2426,7 @@
         <v>73</v>
       </c>
       <c r="B3" t="s">
-        <v>81</v>
+        <v>89</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.35">
@@ -2225,88 +2434,6 @@
         <v>74</v>
       </c>
       <c r="B4" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A5" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="B5" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A6" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="B6" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A7" s="2" t="s">
-        <v>78</v>
-      </c>
-      <c r="B7" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A8" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="B8" t="s">
-        <v>86</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet32.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <cols>
-    <col min="2" max="2" width="11.7265625" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A1" s="10" t="s">
-        <v>71</v>
-      </c>
-      <c r="B1" s="10" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A2" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="B2" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A3" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="B3" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A4" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="B4" t="s">
         <v>90</v>
       </c>
     </row>
@@ -2320,8 +2447,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2358,6 +2485,74 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="10.81640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.54296875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.1796875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A1" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>126</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>127</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A2" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="B2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" t="s">
+        <v>128</v>
+      </c>
+      <c r="D2" t="s">
+        <v>129</v>
+      </c>
+      <c r="E2" t="s">
+        <v>131</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D2"/>
   <sheetViews>
@@ -2409,7 +2604,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E4"/>
   <sheetViews>
@@ -2505,7 +2700,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C4"/>
   <sheetViews>
@@ -2572,108 +2767,4 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B5"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <cols>
-    <col min="1" max="1" width="5.453125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A1" s="4" t="s">
-        <v>71</v>
-      </c>
-      <c r="B1" s="4" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A2" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="B2" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A3" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="B3" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A4" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="B4" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A5" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="B5" t="s">
-        <v>102</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B3"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <cols>
-    <col min="1" max="1" width="5.453125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.81640625" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A1" s="4" t="s">
-        <v>71</v>
-      </c>
-      <c r="B1" s="4" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A2" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="B2" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A3" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="B3" t="s">
-        <v>119</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
update testcases with behavior pwa
</commit_message>
<xml_diff>
--- a/src/main/java/data/data_test.xlsx
+++ b/src/main/java/data/data_test.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7450" firstSheet="1" activeTab="5"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7450" firstSheet="16" activeTab="19"/>
   </bookViews>
   <sheets>
     <sheet name="Login_Success" sheetId="15" r:id="rId1"/>
@@ -107,9 +107,6 @@
     <t>dixosgadpoyt@gmail.com</t>
   </si>
   <si>
-    <t>628229098776544</t>
-  </si>
-  <si>
     <t>Element</t>
   </si>
   <si>
@@ -456,6 +453,9 @@
   </si>
   <si>
     <t>Country Name</t>
+  </si>
+  <si>
+    <t>82290987765</t>
   </si>
 </sst>
 </file>
@@ -885,42 +885,42 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" s="4" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B3" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B4" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" s="2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B5" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
   </sheetData>
@@ -945,26 +945,26 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" s="4" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B2" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B3" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
   </sheetData>
@@ -989,34 +989,34 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" s="4" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B3" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B4" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
   </sheetData>
@@ -1040,50 +1040,50 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" s="4" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B2" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B3" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B4" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" s="2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B5" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" s="2" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B6" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
   </sheetData>
@@ -1108,68 +1108,68 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" s="4" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B2" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B3" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C3" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B4" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C4" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5" s="2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B5" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C5" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A6" s="2" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B6" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C6" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
   </sheetData>
@@ -1193,46 +1193,46 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" s="4" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C2" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B3" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C3" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B4" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C4" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
   </sheetData>
@@ -1266,10 +1266,10 @@
         <v>1</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="E1" s="4" t="s">
         <v>7</v>
@@ -1277,19 +1277,19 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B2" t="s">
         <v>3</v>
       </c>
       <c r="C2" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
   </sheetData>
@@ -1312,50 +1312,50 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" s="4" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" s="8" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" s="8" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" s="8" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B4" s="9" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" s="8" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B5" s="9" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" s="8" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B6" s="9" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
   </sheetData>
@@ -1513,8 +1513,8 @@
   <sheetPr codeName="Sheet3"/>
   <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I14" sqref="I14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1548,7 +1548,7 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
-        <v>16</v>
+        <v>132</v>
       </c>
       <c r="B3" t="s">
         <v>10</v>
@@ -1581,46 +1581,46 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B1" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="C1" s="4" t="s">
         <v>18</v>
-      </c>
-      <c r="C1" s="4" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" s="5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B2" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="C2" s="5" t="s">
         <v>20</v>
-      </c>
-      <c r="C2" s="5" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" s="5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B3" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="C3" s="5" t="s">
         <v>20</v>
-      </c>
-      <c r="C3" s="5" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="29" x14ac:dyDescent="0.35">
       <c r="A4" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B4" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="C4" s="5" t="s">
         <v>20</v>
-      </c>
-      <c r="C4" s="5" t="s">
-        <v>21</v>
       </c>
     </row>
   </sheetData>
@@ -1645,7 +1645,7 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B1" s="4" t="s">
         <v>7</v>
@@ -1653,34 +1653,34 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
   </sheetData>
@@ -1706,13 +1706,13 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" s="4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B1" s="4" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D1" s="4" t="s">
         <v>7</v>
@@ -1723,24 +1723,24 @@
         <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
+        <v>34</v>
+      </c>
+      <c r="B3" t="s">
         <v>35</v>
       </c>
-      <c r="B3" t="s">
-        <v>36</v>
-      </c>
       <c r="C3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D3" t="s">
         <v>9</v>
@@ -1772,13 +1772,13 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" s="4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B1" s="4" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D1" s="4" t="s">
         <v>7</v>
@@ -1786,16 +1786,16 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B2" t="s">
+        <v>38</v>
+      </c>
+      <c r="C2" t="s">
+        <v>38</v>
+      </c>
+      <c r="D2" t="s">
         <v>39</v>
-      </c>
-      <c r="C2" t="s">
-        <v>39</v>
-      </c>
-      <c r="D2" t="s">
-        <v>40</v>
       </c>
     </row>
   </sheetData>
@@ -1824,13 +1824,13 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" s="4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B1" s="4" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D1" s="4" t="s">
         <v>7</v>
@@ -1838,16 +1838,16 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C2" t="s">
+        <v>40</v>
+      </c>
+      <c r="D2" t="s">
         <v>41</v>
-      </c>
-      <c r="D2" t="s">
-        <v>42</v>
       </c>
     </row>
   </sheetData>
@@ -1876,13 +1876,13 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" s="4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B1" s="4" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D1" s="4" t="s">
         <v>7</v>
@@ -1890,16 +1890,16 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" s="6" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C2" t="s">
+        <v>40</v>
+      </c>
+      <c r="D2" t="s">
         <v>41</v>
-      </c>
-      <c r="D2" t="s">
-        <v>42</v>
       </c>
     </row>
   </sheetData>
@@ -1928,13 +1928,13 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" s="4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B1" s="4" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D1" s="4" t="s">
         <v>7</v>
@@ -1942,16 +1942,16 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" s="6" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B2" t="s">
+        <v>38</v>
+      </c>
+      <c r="C2" t="s">
+        <v>38</v>
+      </c>
+      <c r="D2" t="s">
         <v>39</v>
-      </c>
-      <c r="C2" t="s">
-        <v>39</v>
-      </c>
-      <c r="D2" t="s">
-        <v>40</v>
       </c>
     </row>
   </sheetData>
@@ -1980,13 +1980,13 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" s="4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B1" s="4" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D1" s="4" t="s">
         <v>7</v>
@@ -1994,13 +1994,13 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D2" t="s">
         <v>14</v>
@@ -2008,16 +2008,16 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
   </sheetData>
@@ -2037,17 +2037,17 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A1" s="7" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
   </sheetData>
@@ -2070,26 +2070,26 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" s="4" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B2" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B3" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
   </sheetData>
@@ -2114,7 +2114,7 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" s="4" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B1" s="4" t="s">
         <v>0</v>
@@ -2123,15 +2123,15 @@
         <v>1</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E1" s="4" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>2</v>
@@ -2140,15 +2140,15 @@
         <v>3</v>
       </c>
       <c r="D2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>2</v>
@@ -2157,15 +2157,15 @@
         <v>3</v>
       </c>
       <c r="D3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>2</v>
@@ -2174,15 +2174,15 @@
         <v>3</v>
       </c>
       <c r="D4" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E4" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>2</v>
@@ -2191,10 +2191,10 @@
         <v>3</v>
       </c>
       <c r="D5" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E5" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
   </sheetData>
@@ -2271,7 +2271,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B2" t="s">
         <v>9</v>
@@ -2279,7 +2279,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B3" t="s">
         <v>14</v>
@@ -2287,7 +2287,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B4" t="s">
         <v>12</v>
@@ -2295,7 +2295,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B5" t="s">
         <v>12</v>
@@ -2325,66 +2325,66 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" s="10" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B1" s="10" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B3" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B4" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" s="2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B5" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" s="2" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B6" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A7" s="2" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B7" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A8" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B8" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
   </sheetData>
@@ -2407,34 +2407,34 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" s="10" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B1" s="10" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B2" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B3" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B4" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
   </sheetData>
@@ -2458,24 +2458,24 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" s="4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C2" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
   </sheetData>
@@ -2500,7 +2500,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
@@ -2520,30 +2520,30 @@
         <v>1</v>
       </c>
       <c r="C1" s="4" t="s">
+        <v>125</v>
+      </c>
+      <c r="D1" s="4" t="s">
         <v>126</v>
       </c>
-      <c r="D1" s="4" t="s">
-        <v>127</v>
-      </c>
       <c r="E1" s="4" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B2" t="s">
         <v>3</v>
       </c>
       <c r="C2" t="s">
+        <v>127</v>
+      </c>
+      <c r="D2" t="s">
         <v>128</v>
       </c>
-      <c r="D2" t="s">
-        <v>129</v>
-      </c>
       <c r="E2" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
   </sheetData>
@@ -2576,24 +2576,24 @@
         <v>1</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B2" t="s">
         <v>3</v>
       </c>
       <c r="C2" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D2" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
   </sheetData>
@@ -2629,10 +2629,10 @@
         <v>1</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="E1" s="4" t="s">
         <v>7</v>
@@ -2640,50 +2640,50 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B2" t="s">
         <v>3</v>
       </c>
       <c r="C2" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D2" t="s">
         <v>3</v>
       </c>
       <c r="E2" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B3" t="s">
         <v>3</v>
       </c>
       <c r="C3" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>2</v>
       </c>
       <c r="E3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B4" t="s">
         <v>3</v>
       </c>
       <c r="C4" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E4" t="s">
         <v>9</v>
@@ -2723,40 +2723,40 @@
         <v>1</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B2" t="s">
         <v>3</v>
       </c>
       <c r="C2" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B3" t="s">
         <v>3</v>
       </c>
       <c r="C3" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B4" t="s">
         <v>3</v>
       </c>
       <c r="C4" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update testcases Search Home
</commit_message>
<xml_diff>
--- a/src/main/java/data/data_test.xlsx
+++ b/src/main/java/data/data_test.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7450" firstSheet="30" activeTab="30"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7450" firstSheet="27" activeTab="30"/>
   </bookViews>
   <sheets>
     <sheet name="Login_Success" sheetId="15" r:id="rId1"/>
@@ -47,6 +47,11 @@
     <sheet name="Forget_Password_Alert" sheetId="31" r:id="rId33"/>
     <sheet name="List_Tab_Menu_Exclusive" sheetId="34" r:id="rId34"/>
     <sheet name="News_Default_Kanal" sheetId="36" r:id="rId35"/>
+    <sheet name="Menu_Pilar_Tampil" sheetId="57" r:id="rId36"/>
+    <sheet name="Menu_Pilar_Not" sheetId="58" r:id="rId37"/>
+    <sheet name="Pilar" sheetId="59" r:id="rId38"/>
+    <sheet name="News_Content" sheetId="61" r:id="rId39"/>
+    <sheet name="Tab Search" sheetId="62" r:id="rId40"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -58,7 +63,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="336" uniqueCount="135">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="370" uniqueCount="160">
   <si>
     <t>Username</t>
   </si>
@@ -463,6 +468,81 @@
   </si>
   <si>
     <t>tukang ojek pengkolan</t>
+  </si>
+  <si>
+    <t>Menu Id</t>
+  </si>
+  <si>
+    <t>action-home</t>
+  </si>
+  <si>
+    <t>action-live-event</t>
+  </si>
+  <si>
+    <t>action-library</t>
+  </si>
+  <si>
+    <t>Menu</t>
+  </si>
+  <si>
+    <t>action-live-tv</t>
+  </si>
+  <si>
+    <t>action-account</t>
+  </si>
+  <si>
+    <t>Pilar</t>
+  </si>
+  <si>
+    <t>Videos</t>
+  </si>
+  <si>
+    <t>Radio +</t>
+  </si>
+  <si>
+    <t>Home of Talent</t>
+  </si>
+  <si>
+    <t>Games</t>
+  </si>
+  <si>
+    <t>Direct</t>
+  </si>
+  <si>
+    <t>/</t>
+  </si>
+  <si>
+    <t>/trending</t>
+  </si>
+  <si>
+    <t>/radio</t>
+  </si>
+  <si>
+    <t>rc-ugctalent.rctiplus.com</t>
+  </si>
+  <si>
+    <t>/games</t>
+  </si>
+  <si>
+    <t>article-thumbnail</t>
+  </si>
+  <si>
+    <t>Content</t>
+  </si>
+  <si>
+    <t>add-tab-button</t>
+  </si>
+  <si>
+    <t>Tab Search</t>
+  </si>
+  <si>
+    <t>Program</t>
+  </si>
+  <si>
+    <t>Episode</t>
+  </si>
+  <si>
+    <t>Extra</t>
   </si>
 </sst>
 </file>
@@ -2221,7 +2301,7 @@
   <dimension ref="A1:A2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2479,6 +2559,180 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet36.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:A4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K14" sqref="K14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="14.7265625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1" s="10" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>138</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet37.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:A3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G4" sqref="G4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="13.1796875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1" s="10" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>141</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet38.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H11" sqref="H11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="13.7265625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21.6328125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A1" s="10" t="s">
+        <v>142</v>
+      </c>
+      <c r="B1" s="10" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>143</v>
+      </c>
+      <c r="B2" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>82</v>
+      </c>
+      <c r="B3" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>144</v>
+      </c>
+      <c r="B4" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>145</v>
+      </c>
+      <c r="B5" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>146</v>
+      </c>
+      <c r="B6" t="s">
+        <v>152</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet39.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:A3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="15.1796875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1" s="10" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>155</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C2"/>
@@ -2512,6 +2766,73 @@
       </c>
       <c r="C2" t="s">
         <v>123</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet40.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F13" sqref="F13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="2" width="9.90625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A1" s="10" t="s">
+        <v>69</v>
+      </c>
+      <c r="B1" s="10" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A2" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="B2" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A3" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="B3" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A4" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="B4" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A5" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="B5" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A6" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="B6" t="s">
+        <v>80</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
change valeu menu tengah
</commit_message>
<xml_diff>
--- a/src/main/java/data/data_test.xlsx
+++ b/src/main/java/data/data_test.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7450" firstSheet="27" activeTab="30"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7450" firstSheet="12" activeTab="14"/>
   </bookViews>
   <sheets>
     <sheet name="Login_Success" sheetId="15" r:id="rId1"/>
@@ -48,7 +48,7 @@
     <sheet name="List_Tab_Menu_Exclusive" sheetId="34" r:id="rId34"/>
     <sheet name="News_Default_Kanal" sheetId="36" r:id="rId35"/>
     <sheet name="Menu_Pilar_Tampil" sheetId="57" r:id="rId36"/>
-    <sheet name="Menu_Pilar_Not" sheetId="58" r:id="rId37"/>
+    <sheet name="Menu_Pilar_Tak_Tampil" sheetId="58" r:id="rId37"/>
     <sheet name="Pilar" sheetId="59" r:id="rId38"/>
     <sheet name="News_Content" sheetId="61" r:id="rId39"/>
     <sheet name="Tab Search" sheetId="62" r:id="rId40"/>
@@ -63,7 +63,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="370" uniqueCount="160">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="370" uniqueCount="159">
   <si>
     <t>Username</t>
   </si>
@@ -374,9 +374,6 @@
     <t>Exclusive</t>
   </si>
   <si>
-    <t>Radio+</t>
-  </si>
-  <si>
     <t>Home</t>
   </si>
   <si>
@@ -410,12 +407,6 @@
     <t>exclusive</t>
   </si>
   <si>
-    <t>trending</t>
-  </si>
-  <si>
-    <t>radio</t>
-  </si>
-  <si>
     <t>Catch Up TV</t>
   </si>
   <si>
@@ -543,6 +534,12 @@
   </si>
   <si>
     <t>Extra</t>
+  </si>
+  <si>
+    <t>Drama</t>
+  </si>
+  <si>
+    <t>Comedy</t>
   </si>
 </sst>
 </file>
@@ -1043,7 +1040,7 @@
         <v>70</v>
       </c>
       <c r="B2" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
@@ -1051,7 +1048,7 @@
         <v>71</v>
       </c>
       <c r="B3" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
     </row>
   </sheetData>
@@ -1065,7 +1062,7 @@
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:B4"/>
+      <selection activeCell="B2" sqref="B2:B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1095,7 +1092,7 @@
         <v>71</v>
       </c>
       <c r="B3" t="s">
-        <v>82</v>
+        <v>157</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.35">
@@ -1103,7 +1100,7 @@
         <v>72</v>
       </c>
       <c r="B4" t="s">
-        <v>103</v>
+        <v>158</v>
       </c>
     </row>
   </sheetData>
@@ -1138,7 +1135,7 @@
         <v>70</v>
       </c>
       <c r="B2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
@@ -1146,7 +1143,7 @@
         <v>71</v>
       </c>
       <c r="B3" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.35">
@@ -1162,7 +1159,7 @@
         <v>73</v>
       </c>
       <c r="B5" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.35">
@@ -1170,7 +1167,7 @@
         <v>74</v>
       </c>
       <c r="B6" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
   </sheetData>
@@ -1201,7 +1198,7 @@
         <v>101</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.35">
@@ -1209,10 +1206,10 @@
         <v>70</v>
       </c>
       <c r="B2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.35">
@@ -1220,10 +1217,10 @@
         <v>71</v>
       </c>
       <c r="B3" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C3" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.35">
@@ -1234,7 +1231,7 @@
         <v>51</v>
       </c>
       <c r="C4" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.35">
@@ -1242,10 +1239,10 @@
         <v>73</v>
       </c>
       <c r="B5" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C5" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.35">
@@ -1253,10 +1250,10 @@
         <v>74</v>
       </c>
       <c r="B6" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C6" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
   </sheetData>
@@ -1268,8 +1265,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J9" sqref="J9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1286,7 +1283,7 @@
         <v>101</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.35">
@@ -1297,7 +1294,7 @@
         <v>102</v>
       </c>
       <c r="C2" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.35">
@@ -1305,10 +1302,10 @@
         <v>71</v>
       </c>
       <c r="B3" t="s">
-        <v>82</v>
+        <v>157</v>
       </c>
       <c r="C3" t="s">
-        <v>115</v>
+        <v>157</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.35">
@@ -1316,10 +1313,10 @@
         <v>72</v>
       </c>
       <c r="B4" t="s">
-        <v>103</v>
+        <v>158</v>
       </c>
       <c r="C4" t="s">
-        <v>116</v>
+        <v>158</v>
       </c>
     </row>
   </sheetData>
@@ -1635,7 +1632,7 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="B3" t="s">
         <v>10</v>
@@ -2160,7 +2157,7 @@
         <v>69</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">
@@ -2168,7 +2165,7 @@
         <v>70</v>
       </c>
       <c r="B2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
@@ -2176,7 +2173,7 @@
         <v>71</v>
       </c>
       <c r="B3" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
     </row>
   </sheetData>
@@ -2227,7 +2224,7 @@
         <v>3</v>
       </c>
       <c r="D2" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="E2" t="s">
         <v>53</v>
@@ -2244,7 +2241,7 @@
         <v>3</v>
       </c>
       <c r="D3" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="E3" t="s">
         <v>53</v>
@@ -2261,7 +2258,7 @@
         <v>3</v>
       </c>
       <c r="D4" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="E4" t="s">
         <v>53</v>
@@ -2278,7 +2275,7 @@
         <v>3</v>
       </c>
       <c r="D5" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="E5" t="s">
         <v>53</v>
@@ -2300,7 +2297,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
@@ -2311,12 +2308,12 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A1" s="4" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
     </row>
   </sheetData>
@@ -2564,7 +2561,7 @@
   <dimension ref="A1:A4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K14" sqref="K14"/>
+      <selection activeCell="K6" sqref="K6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2574,22 +2571,22 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A1" s="10" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
     </row>
   </sheetData>
@@ -2603,7 +2600,7 @@
   <dimension ref="A1:A3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+      <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2613,17 +2610,17 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A1" s="10" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
     </row>
   </sheetData>
@@ -2647,18 +2644,18 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" s="10" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="B1" s="10" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="B2" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
@@ -2666,31 +2663,31 @@
         <v>82</v>
       </c>
       <c r="B3" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="B4" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="B5" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="B6" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
     </row>
   </sheetData>
@@ -2714,17 +2711,17 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A1" s="10" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
     </row>
   </sheetData>
@@ -2754,18 +2751,18 @@
         <v>69</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>76</v>
       </c>
       <c r="C2" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
     </row>
   </sheetData>
@@ -2792,7 +2789,7 @@
         <v>69</v>
       </c>
       <c r="B1" s="10" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">
@@ -2800,7 +2797,7 @@
         <v>70</v>
       </c>
       <c r="B2" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
@@ -2808,7 +2805,7 @@
         <v>71</v>
       </c>
       <c r="B3" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.35">
@@ -2816,7 +2813,7 @@
         <v>72</v>
       </c>
       <c r="B4" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.35">
@@ -2877,30 +2874,30 @@
         <v>1</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="E1" s="4" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="B2" t="s">
         <v>3</v>
       </c>
       <c r="C2" t="s">
+        <v>123</v>
+      </c>
+      <c r="D2" t="s">
+        <v>124</v>
+      </c>
+      <c r="E2" t="s">
         <v>126</v>
-      </c>
-      <c r="D2" t="s">
-        <v>127</v>
-      </c>
-      <c r="E2" t="s">
-        <v>129</v>
       </c>
     </row>
   </sheetData>

</xml_diff>